<commit_message>
Se actualiza funcion de utilidades
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otobismac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otobismac/Coverflow-JS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{DC817442-BD16-6745-A0B9-5F1BF1848519}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907BC653-0628-0E41-8E6D-084AB26F4884}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{F997655D-7DCE-784F-A080-90DDDFA7AF1C}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>prima vacacional</t>
   </si>
   <si>
-    <t>DIFF</t>
+    <t>DIF</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Se ajusta archivo Excel
</commit_message>
<xml_diff>
--- a/Calculos.xlsx
+++ b/Calculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/otobismac/Coverflow-JS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907BC653-0628-0E41-8E6D-084AB26F4884}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEAC233-87ED-5346-BBA0-C0CDAAD49A6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{F997655D-7DCE-784F-A080-90DDDFA7AF1C}"/>
   </bookViews>
@@ -51,7 +51,7 @@
     <t>prima vacacional</t>
   </si>
   <si>
-    <t>DIF</t>
+    <t>DIFF</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>